<commit_message>
Added p2processanalyse and peter-assesments
</commit_message>
<xml_diff>
--- a/files/assesments/firstround/assesments-peter.xlsx
+++ b/files/assesments/firstround/assesments-peter.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobvejlinjensen/Honeyjar/files/assesments/firstround/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piiit\Documents\Honeyjar\files\assesments\firstround\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E543199-7360-4C0B-A7CB-7D848705B0B9}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20500" windowHeight="7540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20500" windowHeight="7540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Peer  and self assessment" sheetId="2" r:id="rId1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
   <si>
     <t>Self assesment</t>
   </si>
@@ -103,12 +104,39 @@
   </si>
   <si>
     <t>Alex</t>
+  </si>
+  <si>
+    <t>Self assesment (Peter)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good use of communication programs, and making sure everybody is on the right track. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Very motivated. Asking everyone where we are in the project, and what needs to be done. </t>
+  </si>
+  <si>
+    <t>Guiding everyone on how to use the programs (github/sourcetree etc..) very helpful and good overview.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Same as Ahmed. Asking relevant questions and keeping close contact. </t>
+  </si>
+  <si>
+    <t>Keeping close contact, and bringing a lot of ideas to the table.</t>
+  </si>
+  <si>
+    <t>Keeping contact and helps create overall overview of the project.</t>
+  </si>
+  <si>
+    <t>Haven't participated at all.</t>
+  </si>
+  <si>
+    <t>Keeping close contact (asking/responding when needed). Also very motivated and helps keeping an overview</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -282,10 +310,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:A5" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
-  <autoFilter ref="A1:A5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:A5" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+  <autoFilter ref="A1:A5" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Grade" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Grade" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -553,14 +581,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="40.1640625" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" customWidth="1"/>
@@ -568,7 +596,7 @@
     <col min="7" max="7" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
@@ -579,78 +607,114 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
-    </row>
-    <row r="3" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
-    </row>
-    <row r="5" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="13" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>9</v>
       </c>
@@ -661,99 +725,99 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="9"/>
     </row>
-    <row r="28" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="9"/>
     </row>
-    <row r="29" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>13</v>
       </c>
@@ -767,14 +831,14 @@
     <mergeCell ref="B29:C29"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Give at least two examples" sqref="C2:C11 C15:C24"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Give at least two examples" sqref="C2:C11 C15:C24" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose a grade">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose a grade" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>Sheet1!$A$2:$A$5</xm:f>
           </x14:formula1>
@@ -787,19 +851,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -810,7 +874,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -821,7 +885,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -832,7 +896,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -843,7 +907,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -854,7 +918,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -863,7 +927,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -872,7 +936,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -881,7 +945,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -890,7 +954,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -899,7 +963,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -908,7 +972,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -917,7 +981,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -926,7 +990,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -935,7 +999,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -944,7 +1008,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -953,7 +1017,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -962,7 +1026,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -971,7 +1035,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -980,7 +1044,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -989,7 +1053,7 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -998,7 +1062,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1007,7 +1071,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>

</xml_diff>